<commit_message>
this is selenium examples project update 5 oct 25
</commit_message>
<xml_diff>
--- a/DataDriven/ScanOnline_LoginData_DataDrivenTest.xlsx
+++ b/DataDriven/ScanOnline_LoginData_DataDrivenTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\eclipse-workspace\Java\.metadata\.metadata\SeleniumAutomationExamples\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCC95CCD-40B2-465F-97A2-97B2A657551D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AD642A-1C0E-4EEA-BF76-467BF7D9040C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,12 +36,6 @@
     <t>res</t>
   </si>
   <si>
-    <t>YuvrajScan</t>
-  </si>
-  <si>
-    <t>Admin@2029</t>
-  </si>
-  <si>
     <t>valid</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>GoodQa@123</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -377,62 +377,62 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="Admin@2029" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>

</xml_diff>